<commit_message>
Pushing Generator for all list
</commit_message>
<xml_diff>
--- a/Employee-Management-System/employeeList.xlsx
+++ b/Employee-Management-System/employeeList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Employee ID</t>
   </si>
@@ -78,72 +78,6 @@
   </si>
   <si>
     <t>ADMIN</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>SRIKHAR EDARA</t>
-  </si>
-  <si>
-    <t>eone</t>
-  </si>
-  <si>
-    <t>1996-06-14</t>
-  </si>
-  <si>
-    <t>ENGINEER -- DELHI</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>ABHISHEK NIM</t>
-  </si>
-  <si>
-    <t>etwo</t>
-  </si>
-  <si>
-    <t>2022-05-04</t>
-  </si>
-  <si>
-    <t>1997-11-29</t>
-  </si>
-  <si>
-    <t>IDEA PARK -- BANGALORE</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>YASHVI MANIAR</t>
-  </si>
-  <si>
-    <t>ykm</t>
-  </si>
-  <si>
-    <t>2022-05-25</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>2001-06-06</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>SOHAM SHARMA</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>2022-05-11</t>
-  </si>
-  <si>
-    <t>1999-02-08</t>
   </si>
 </sst>
 </file>
@@ -195,20 +129,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="12.04296875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="15.828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="15.0546875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.796875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="12.44140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.8359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="7.453125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.44140625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="10.16015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="24.51953125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="21.140625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -289,110 +223,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>